<commit_message>
test 10.2 almost ready + update of lesson 5.2. Objects_02b
</commit_message>
<xml_diff>
--- a/cs3e/Ex/MazpenHelekGimel.xlsx
+++ b/cs3e/Ex/MazpenHelekGimel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\stra\repos\BeautifulYesodot\cs3e\Ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8C3A5B-4126-4218-BDBE-87188DC82CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A90CC6-BBFD-40A2-AF61-984A159D3BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,7 +823,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1052,13 +1052,16 @@
       <c r="L5">
         <v>1</v>
       </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="S5" s="4"/>
       <c r="X5">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -1078,6 +1081,9 @@
         <v>1</v>
       </c>
       <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
       <c r="N6" s="4"/>
@@ -1086,7 +1092,7 @@
       <c r="S6" s="4"/>
       <c r="X6">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -1109,6 +1115,9 @@
         <v>1</v>
       </c>
       <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
         <v>1</v>
       </c>
       <c r="N7" s="4"/>
@@ -1117,7 +1126,7 @@
       <c r="S7" s="4"/>
       <c r="X7">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -1132,9 +1141,6 @@
       </c>
       <c r="I8">
         <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
       </c>
       <c r="K8" s="4">
         <v>1</v>
@@ -1164,9 +1170,6 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9" s="4">
         <v>0.5</v>
       </c>
@@ -1183,21 +1186,8 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
+      <c r="H10" s="4"/>
+      <c r="K10" s="4"/>
       <c r="N10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1217,15 +1207,7 @@
       <c r="H11" s="4">
         <v>0.5</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
+      <c r="K11" s="4"/>
       <c r="N11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1251,10 +1233,11 @@
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
+      <c r="K12" s="4"/>
       <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>1</v>
       </c>
       <c r="N12" s="4"/>
@@ -1263,7 +1246,7 @@
       <c r="S12" s="4"/>
       <c r="X12">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
@@ -1283,6 +1266,12 @@
         <v>1</v>
       </c>
       <c r="K13" s="4">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" s="4"/>
@@ -1291,7 +1280,7 @@
       <c r="S13" s="4"/>
       <c r="X13">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -1311,6 +1300,9 @@
         <v>1</v>
       </c>
       <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <v>1</v>
       </c>
       <c r="N14" s="4"/>
@@ -1319,7 +1311,7 @@
       <c r="S14" s="4"/>
       <c r="X14">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -1339,6 +1331,9 @@
         <v>1</v>
       </c>
       <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15">
         <v>1</v>
       </c>
       <c r="N15" s="4"/>
@@ -1347,7 +1342,7 @@
       <c r="S15" s="4"/>
       <c r="X15">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -1366,10 +1361,11 @@
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
+      <c r="K16" s="4"/>
       <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
         <v>1</v>
       </c>
       <c r="N16" s="4"/>
@@ -1378,7 +1374,7 @@
       <c r="S16" s="4"/>
       <c r="X16">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
@@ -1398,6 +1394,12 @@
         <v>1</v>
       </c>
       <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
         <v>1</v>
       </c>
       <c r="N17" s="4"/>
@@ -1406,7 +1408,7 @@
       <c r="S17" s="4"/>
       <c r="X17">
         <f>SUM(טבלה3[[#This Row],[Thu 1/1]:[ספייר]])</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>